<commit_message>
Update Travel details dataset.xlsx
</commit_message>
<xml_diff>
--- a/Travel details dataset.xlsx
+++ b/Travel details dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roni0\שולחן העבודה\ruppin\פרוייקט גמר מערכות מידע\aravaTrip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2E5160-118E-4AE9-9C5E-CBE9CCDBF71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E687C2-D770-4409-A409-C32B72145B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Travel details dataset משהו נדפ" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2413" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2444" uniqueCount="280">
   <si>
     <t>Trip ID</t>
   </si>
@@ -830,10 +830,37 @@
     <t>Indian Airlines</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>Iberia</t>
+  </si>
+  <si>
+    <t>Garuda Indonesia</t>
+  </si>
+  <si>
+    <t>Royal Air Maroc</t>
+  </si>
+  <si>
+    <t>Japan Airlines</t>
+  </si>
+  <si>
+    <t>China Airlines</t>
+  </si>
+  <si>
+    <t>Korean Air</t>
+  </si>
+  <si>
+    <t>Sun BusAir Chaiyaphum</t>
+  </si>
+  <si>
+    <t>Toei Bus</t>
+  </si>
+  <si>
+    <t>Charter Buses Toronto</t>
+  </si>
+  <si>
+    <t>Brasil Bus Travel</t>
+  </si>
+  <si>
+    <t>Greyhound </t>
   </si>
 </sst>
 </file>
@@ -1341,7 +1368,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1352,6 +1379,12 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - הדגשה1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1790,7 +1823,7 @@
   <sheetPr codeName="Worksheet______1"/>
   <dimension ref="A1:Y138"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R69" sqref="R69"/>
     </sheetView>
   </sheetViews>
@@ -10971,30 +11004,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A868E4-A452-413C-97A1-644A92D3AC65}">
-  <dimension ref="A1:U138"/>
+  <dimension ref="A1:V138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B2:B7"/>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="24.25" customWidth="1"/>
-    <col min="3" max="3" width="12.1875" hidden="1" customWidth="1"/>
-    <col min="4" max="8" width="12.25" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="9" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="7.625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="16.875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="11" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.75" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.25" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="13.375" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.75" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9" customWidth="1"/>
-    <col min="21" max="21" width="8.75" customWidth="1"/>
+    <col min="3" max="3" width="12.1875" customWidth="1"/>
+    <col min="4" max="8" width="12.25" customWidth="1"/>
+    <col min="9" max="9" width="13.5" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="7.625" customWidth="1"/>
+    <col min="12" max="12" width="16.875" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="13.75" customWidth="1"/>
+    <col min="15" max="15" width="18.375" customWidth="1"/>
+    <col min="16" max="16" width="7.25" customWidth="1"/>
+    <col min="17" max="17" width="13.375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="21.4375" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.875" customWidth="1"/>
+    <col min="20" max="20" width="27.75" customWidth="1"/>
+    <col min="21" max="21" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -11049,17 +11082,17 @@
       <c r="Q1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="R1" t="s">
-        <v>229</v>
+      <c r="R1" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="T1" t="s">
+        <v>229</v>
+      </c>
+      <c r="U1" t="s">
         <v>10</v>
-      </c>
-      <c r="U1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -11114,15 +11147,17 @@
       <c r="Q2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="7">
+        <v>4</v>
+      </c>
+      <c r="S2" t="s">
         <v>81</v>
       </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="U2">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -11177,15 +11212,17 @@
       <c r="Q3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="7">
+        <v>5</v>
+      </c>
+      <c r="S3" t="s">
         <v>81</v>
       </c>
-      <c r="S3" s="4"/>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="U3">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -11240,15 +11277,17 @@
       <c r="Q4" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="S4" t="s">
         <v>81</v>
       </c>
-      <c r="S4" s="4"/>
-      <c r="T4" s="1" t="s">
+      <c r="T4" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="U4">
-        <v>2.5</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -11303,15 +11342,17 @@
       <c r="Q5" s="3">
         <v>500</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="7">
+        <v>5</v>
+      </c>
+      <c r="S5" t="s">
         <v>81</v>
       </c>
-      <c r="S5" s="4"/>
-      <c r="T5" s="1">
+      <c r="T5" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="U5" s="1">
         <v>50</v>
-      </c>
-      <c r="U5">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -11366,15 +11407,17 @@
       <c r="Q6" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="S6" t="s">
         <v>81</v>
       </c>
-      <c r="S6" s="4"/>
-      <c r="T6" s="1" t="s">
+      <c r="T6" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="U6">
-        <v>3.5</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -11429,15 +11472,17 @@
       <c r="Q7" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="S7" t="s">
         <v>81</v>
       </c>
-      <c r="S7" s="4"/>
-      <c r="T7" s="1" t="s">
+      <c r="T7" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="U7">
-        <v>3.5</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -11492,17 +11537,17 @@
       <c r="Q8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" s="7">
+        <v>5</v>
+      </c>
+      <c r="S8" t="s">
         <v>105</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="T8" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="U8">
-        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -11557,17 +11602,17 @@
       <c r="Q9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="7">
+        <v>5</v>
+      </c>
+      <c r="S9" t="s">
         <v>105</v>
       </c>
-      <c r="S9" s="4" t="s">
+      <c r="T9" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="U9">
-        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -11622,17 +11667,17 @@
       <c r="Q10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10" s="7">
+        <v>5</v>
+      </c>
+      <c r="S10" t="s">
         <v>105</v>
       </c>
-      <c r="S10" s="4" t="s">
+      <c r="T10" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="U10">
-        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -11687,17 +11732,17 @@
       <c r="Q11" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="S11" t="s">
         <v>105</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="T11" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="U11" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="U11">
-        <v>3.5</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -11752,17 +11797,17 @@
       <c r="Q12" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R12" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="S12" t="s">
         <v>105</v>
       </c>
-      <c r="S12" s="4" t="s">
+      <c r="T12" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="U12" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="U12">
-        <v>4.5</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -11817,17 +11862,17 @@
       <c r="Q13" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="S13" t="s">
         <v>105</v>
       </c>
-      <c r="S13" s="4" t="s">
+      <c r="T13" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="U13" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="U13">
-        <v>4.5</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -11882,17 +11927,17 @@
       <c r="Q14" s="3">
         <v>800</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R14" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="S14" t="s">
         <v>105</v>
       </c>
-      <c r="S14" s="4" t="s">
+      <c r="T14" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="T14" s="1">
+      <c r="U14" s="1">
         <v>200</v>
-      </c>
-      <c r="U14">
-        <v>4.5</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -11947,17 +11992,17 @@
       <c r="Q15" s="3">
         <v>400</v>
       </c>
-      <c r="R15" t="s">
+      <c r="R15" s="7">
+        <v>5</v>
+      </c>
+      <c r="S15" t="s">
         <v>105</v>
       </c>
-      <c r="S15" s="4" t="s">
+      <c r="T15" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="T15" s="1">
+      <c r="U15" s="1">
         <v>300</v>
-      </c>
-      <c r="U15">
-        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -12012,17 +12057,17 @@
       <c r="Q16" s="3">
         <v>700</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R16" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="S16" t="s">
         <v>105</v>
       </c>
-      <c r="S16" s="4" t="s">
+      <c r="T16" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="T16" s="1">
+      <c r="U16" s="1">
         <v>200</v>
-      </c>
-      <c r="U16">
-        <v>2.5</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -12077,17 +12122,17 @@
       <c r="Q17" s="3">
         <v>1500</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17" s="7">
+        <v>3</v>
+      </c>
+      <c r="S17" t="s">
         <v>105</v>
       </c>
-      <c r="S17" s="4" t="s">
+      <c r="T17" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="T17" s="1">
+      <c r="U17" s="1">
         <v>300</v>
-      </c>
-      <c r="U17">
-        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -12142,17 +12187,17 @@
       <c r="Q18" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="R18" t="s">
+      <c r="R18" s="7">
+        <v>4</v>
+      </c>
+      <c r="S18" t="s">
         <v>105</v>
       </c>
-      <c r="S18" s="4" t="s">
+      <c r="T18" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="U18" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="U18">
-        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -12207,17 +12252,17 @@
       <c r="Q19" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="R19" t="s">
+      <c r="R19" s="7">
+        <v>4</v>
+      </c>
+      <c r="S19" t="s">
         <v>105</v>
       </c>
-      <c r="S19" s="4" t="s">
+      <c r="T19" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="T19" s="1" t="s">
+      <c r="U19" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="U19">
-        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -12272,17 +12317,17 @@
       <c r="Q20" s="3">
         <v>1200</v>
       </c>
-      <c r="R20" t="s">
+      <c r="R20" s="7">
+        <v>5</v>
+      </c>
+      <c r="S20" t="s">
         <v>105</v>
       </c>
-      <c r="S20" s="4" t="s">
+      <c r="T20" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="T20" s="1">
+      <c r="U20" s="1">
         <v>200</v>
-      </c>
-      <c r="U20">
-        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -12337,17 +12382,17 @@
       <c r="Q21" s="3">
         <v>1500</v>
       </c>
-      <c r="R21" t="s">
+      <c r="R21" s="7">
+        <v>5</v>
+      </c>
+      <c r="S21" t="s">
         <v>105</v>
       </c>
-      <c r="S21" s="4" t="s">
+      <c r="T21" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="T21" s="1">
+      <c r="U21" s="1">
         <v>300</v>
-      </c>
-      <c r="U21">
-        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -12402,17 +12447,17 @@
       <c r="Q22" s="3">
         <v>3000</v>
       </c>
-      <c r="R22" t="s">
+      <c r="R22" s="7">
+        <v>4</v>
+      </c>
+      <c r="S22" t="s">
         <v>105</v>
       </c>
-      <c r="S22" s="4" t="s">
+      <c r="T22" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="T22" s="1">
+      <c r="U22" s="1">
         <v>2000</v>
-      </c>
-      <c r="U22">
-        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -12467,17 +12512,17 @@
       <c r="Q23" s="3">
         <v>2500</v>
       </c>
-      <c r="R23" t="s">
+      <c r="R23" s="7">
+        <v>5</v>
+      </c>
+      <c r="S23" t="s">
         <v>105</v>
       </c>
-      <c r="S23" s="4" t="s">
+      <c r="T23" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="T23" s="1">
+      <c r="U23" s="1">
         <v>2000</v>
-      </c>
-      <c r="U23">
-        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -12532,17 +12577,17 @@
       <c r="Q24" s="3">
         <v>1000</v>
       </c>
-      <c r="R24" t="s">
+      <c r="R24" s="7">
+        <v>5</v>
+      </c>
+      <c r="S24" t="s">
         <v>201</v>
       </c>
-      <c r="S24" s="4" t="s">
+      <c r="T24" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="T24" s="1">
+      <c r="U24" s="1">
         <v>150</v>
-      </c>
-      <c r="U24">
-        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -12597,17 +12642,17 @@
       <c r="Q25" s="3">
         <v>1200</v>
       </c>
-      <c r="R25" t="s">
+      <c r="R25" s="7">
+        <v>3</v>
+      </c>
+      <c r="S25" t="s">
         <v>68</v>
       </c>
-      <c r="S25" s="4" t="s">
+      <c r="T25" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="T25" s="1">
+      <c r="U25" s="1">
         <v>600</v>
-      </c>
-      <c r="U25">
-        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -12662,17 +12707,17 @@
       <c r="Q26" s="3">
         <v>800</v>
       </c>
-      <c r="R26" t="s">
+      <c r="R26" s="7">
+        <v>3</v>
+      </c>
+      <c r="S26" t="s">
         <v>68</v>
       </c>
-      <c r="S26" s="4" t="s">
+      <c r="T26" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="T26" s="1">
+      <c r="U26" s="1">
         <v>500</v>
-      </c>
-      <c r="U26">
-        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.35">
@@ -12727,14 +12772,17 @@
       <c r="Q27" s="3">
         <v>1000</v>
       </c>
-      <c r="R27" t="s">
+      <c r="R27" s="7">
+        <v>3</v>
+      </c>
+      <c r="S27" t="s">
         <v>68</v>
       </c>
-      <c r="T27" s="1">
+      <c r="T27" t="s">
+        <v>270</v>
+      </c>
+      <c r="U27" s="1">
         <v>700</v>
-      </c>
-      <c r="U27">
-        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -12789,17 +12837,17 @@
       <c r="Q28" s="3">
         <v>2000</v>
       </c>
-      <c r="R28" t="s">
+      <c r="R28" s="7">
+        <v>3</v>
+      </c>
+      <c r="S28" t="s">
         <v>68</v>
       </c>
-      <c r="S28" s="4" t="s">
+      <c r="T28" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="T28" s="1">
+      <c r="U28" s="1">
         <v>1000</v>
-      </c>
-      <c r="U28">
-        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -12854,17 +12902,17 @@
       <c r="Q29" s="3">
         <v>1500</v>
       </c>
-      <c r="R29" t="s">
+      <c r="R29" s="7">
+        <v>3</v>
+      </c>
+      <c r="S29" t="s">
         <v>68</v>
       </c>
-      <c r="S29" s="4" t="s">
+      <c r="T29" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="T29" s="1">
+      <c r="U29" s="1">
         <v>800</v>
-      </c>
-      <c r="U29">
-        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -12919,17 +12967,17 @@
       <c r="Q30" s="3">
         <v>500</v>
       </c>
-      <c r="R30" t="s">
+      <c r="R30" s="7">
+        <v>3</v>
+      </c>
+      <c r="S30" t="s">
         <v>68</v>
       </c>
-      <c r="S30" s="4" t="s">
+      <c r="T30" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="T30" s="1">
+      <c r="U30" s="1">
         <v>1200</v>
-      </c>
-      <c r="U30">
-        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -12984,17 +13032,17 @@
       <c r="Q31" s="3">
         <v>900</v>
       </c>
-      <c r="R31" t="s">
+      <c r="R31" s="7">
+        <v>3</v>
+      </c>
+      <c r="S31" t="s">
         <v>68</v>
       </c>
-      <c r="S31" s="4" t="s">
+      <c r="T31" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="T31" s="1">
+      <c r="U31" s="1">
         <v>600</v>
-      </c>
-      <c r="U31">
-        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -13049,17 +13097,17 @@
       <c r="Q32" s="3">
         <v>2500</v>
       </c>
-      <c r="R32" t="s">
+      <c r="R32" s="7">
+        <v>3</v>
+      </c>
+      <c r="S32" t="s">
         <v>68</v>
       </c>
-      <c r="S32" s="4" t="s">
+      <c r="T32" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="T32" s="1">
+      <c r="U32" s="1">
         <v>800</v>
-      </c>
-      <c r="U32">
-        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -13114,17 +13162,17 @@
       <c r="Q33" s="3">
         <v>1000</v>
       </c>
-      <c r="R33" t="s">
+      <c r="R33" s="7">
+        <v>3</v>
+      </c>
+      <c r="S33" t="s">
         <v>68</v>
       </c>
-      <c r="S33" s="4" t="s">
+      <c r="T33" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="T33" s="1">
+      <c r="U33" s="1">
         <v>500</v>
-      </c>
-      <c r="U33">
-        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -13179,17 +13227,17 @@
       <c r="Q34" s="3">
         <v>3000</v>
       </c>
-      <c r="R34" t="s">
+      <c r="R34" s="7">
+        <v>4</v>
+      </c>
+      <c r="S34" t="s">
         <v>68</v>
       </c>
-      <c r="S34" s="4" t="s">
+      <c r="T34" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="T34" s="1">
+      <c r="U34" s="1">
         <v>1200</v>
-      </c>
-      <c r="U34">
-        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -13244,17 +13292,17 @@
       <c r="Q35" s="3">
         <v>1400</v>
       </c>
-      <c r="R35" t="s">
+      <c r="R35" s="7">
+        <v>4</v>
+      </c>
+      <c r="S35" t="s">
         <v>68</v>
       </c>
-      <c r="S35" s="4" t="s">
+      <c r="T35" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="T35" s="1">
+      <c r="U35" s="1">
         <v>700</v>
-      </c>
-      <c r="U35">
-        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -13309,15 +13357,17 @@
       <c r="Q36" s="3">
         <v>600</v>
       </c>
-      <c r="R36" t="s">
+      <c r="R36" s="7">
+        <v>4</v>
+      </c>
+      <c r="S36" t="s">
         <v>68</v>
       </c>
-      <c r="S36" s="4"/>
-      <c r="T36" s="1">
+      <c r="T36" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="U36" s="1">
         <v>400</v>
-      </c>
-      <c r="U36">
-        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -13372,20 +13422,20 @@
       <c r="Q37" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="R37" t="s">
+      <c r="R37" s="7">
+        <v>4</v>
+      </c>
+      <c r="S37" t="s">
         <v>68</v>
       </c>
-      <c r="S37" s="4" t="s">
+      <c r="T37" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="T37" s="1" t="s">
+      <c r="U37" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="U37">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>18</v>
       </c>
@@ -13437,15 +13487,17 @@
       <c r="Q38" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="R38" t="s">
+      <c r="R38" s="7">
+        <v>4</v>
+      </c>
+      <c r="S38" t="s">
         <v>68</v>
       </c>
-      <c r="S38" s="4"/>
-      <c r="T38" s="1" t="s">
+      <c r="T38" t="s">
+        <v>270</v>
+      </c>
+      <c r="U38" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="U38">
-        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -13500,17 +13552,17 @@
       <c r="Q39" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="R39" t="s">
+      <c r="R39" s="7">
+        <v>4</v>
+      </c>
+      <c r="S39" t="s">
         <v>68</v>
       </c>
-      <c r="S39" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="T39" s="1" t="s">
+      <c r="T39" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="U39" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="U39">
-        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -13565,17 +13617,17 @@
       <c r="Q40" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="R40" t="s">
+      <c r="R40" s="7">
+        <v>4</v>
+      </c>
+      <c r="S40" t="s">
         <v>68</v>
       </c>
-      <c r="S40" s="4" t="s">
+      <c r="T40" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="T40" s="1" t="s">
+      <c r="U40" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="U40">
-        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -13630,15 +13682,17 @@
       <c r="Q41" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="R41" t="s">
+      <c r="R41" s="7">
+        <v>4</v>
+      </c>
+      <c r="S41" t="s">
         <v>68</v>
       </c>
-      <c r="S41" s="4"/>
-      <c r="T41" s="1" t="s">
+      <c r="T41" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="U41" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="U41">
-        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -13693,17 +13747,17 @@
       <c r="Q42" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="R42" t="s">
+      <c r="R42" s="7">
+        <v>4</v>
+      </c>
+      <c r="S42" t="s">
         <v>68</v>
       </c>
-      <c r="S42" s="4" t="s">
+      <c r="T42" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="T42" s="1" t="s">
+      <c r="U42" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="U42">
-        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -13758,17 +13812,17 @@
       <c r="Q43" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="R43" t="s">
+      <c r="R43" s="7">
+        <v>5</v>
+      </c>
+      <c r="S43" t="s">
         <v>68</v>
       </c>
-      <c r="S43" s="4" t="s">
+      <c r="T43" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="T43" s="1" t="s">
+      <c r="U43" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="U43">
-        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -13823,17 +13877,17 @@
       <c r="Q44" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="R44" t="s">
+      <c r="R44" s="7">
+        <v>5</v>
+      </c>
+      <c r="S44" t="s">
         <v>68</v>
       </c>
-      <c r="S44" s="4" t="s">
+      <c r="T44" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="T44" s="1" t="s">
+      <c r="U44" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="U44">
-        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -13888,15 +13942,17 @@
       <c r="Q45" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R45" t="s">
+      <c r="R45" s="7">
+        <v>5</v>
+      </c>
+      <c r="S45" t="s">
         <v>68</v>
       </c>
-      <c r="S45" s="4"/>
-      <c r="T45" s="1" t="s">
+      <c r="T45" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="U45" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="U45">
-        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -13951,17 +14007,17 @@
       <c r="Q46" s="3">
         <v>1400</v>
       </c>
-      <c r="R46" t="s">
+      <c r="R46" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="S46" t="s">
         <v>68</v>
       </c>
-      <c r="S46" s="4" t="s">
+      <c r="T46" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="T46" s="1">
+      <c r="U46" s="1">
         <v>600</v>
-      </c>
-      <c r="U46">
-        <v>2.5</v>
       </c>
     </row>
     <row r="47" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14016,15 +14072,17 @@
       <c r="Q47" s="3">
         <v>500</v>
       </c>
-      <c r="R47" t="s">
+      <c r="R47" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="S47" t="s">
         <v>68</v>
       </c>
-      <c r="S47" s="4"/>
-      <c r="T47" s="1">
+      <c r="T47" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="U47" s="1">
         <v>900</v>
-      </c>
-      <c r="U47">
-        <v>2.5</v>
       </c>
     </row>
     <row r="48" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14079,17 +14137,17 @@
       <c r="Q48" s="3">
         <v>2200</v>
       </c>
-      <c r="R48" t="s">
+      <c r="R48" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="S48" t="s">
         <v>68</v>
       </c>
-      <c r="S48" s="4" t="s">
+      <c r="T48" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="T48" s="1">
+      <c r="U48" s="1">
         <v>800</v>
-      </c>
-      <c r="U48">
-        <v>2.5</v>
       </c>
     </row>
     <row r="49" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14144,17 +14202,17 @@
       <c r="Q49" s="3">
         <v>1200</v>
       </c>
-      <c r="R49" t="s">
+      <c r="R49" s="7">
+        <v>5</v>
+      </c>
+      <c r="S49" t="s">
         <v>68</v>
       </c>
-      <c r="S49" s="4" t="s">
+      <c r="T49" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="T49" s="1">
+      <c r="U49" s="1">
         <v>700</v>
-      </c>
-      <c r="U49">
-        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14209,15 +14267,17 @@
       <c r="Q50" s="3">
         <v>600</v>
       </c>
-      <c r="R50" t="s">
+      <c r="R50" s="7">
+        <v>5</v>
+      </c>
+      <c r="S50" t="s">
         <v>68</v>
       </c>
-      <c r="S50" s="4"/>
-      <c r="T50" s="1">
+      <c r="T50" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="U50" s="1">
         <v>600</v>
-      </c>
-      <c r="U50">
-        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14272,17 +14332,17 @@
       <c r="Q51" s="3">
         <v>1500</v>
       </c>
-      <c r="R51" t="s">
+      <c r="R51" s="7">
+        <v>5</v>
+      </c>
+      <c r="S51" t="s">
         <v>68</v>
       </c>
-      <c r="S51" s="4" t="s">
+      <c r="T51" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="T51" s="1">
+      <c r="U51" s="1">
         <v>500</v>
-      </c>
-      <c r="U51">
-        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14337,15 +14397,17 @@
       <c r="Q52" s="3">
         <v>1100</v>
       </c>
-      <c r="R52" t="s">
+      <c r="R52" s="7">
+        <v>5</v>
+      </c>
+      <c r="S52" t="s">
         <v>68</v>
       </c>
-      <c r="S52" s="4"/>
-      <c r="T52" s="1">
+      <c r="T52" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="U52" s="1">
         <v>700</v>
-      </c>
-      <c r="U52">
-        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14400,17 +14462,17 @@
       <c r="Q53" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="R53" t="s">
+      <c r="R53" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="S53" t="s">
         <v>68</v>
       </c>
-      <c r="S53" s="4" t="s">
+      <c r="T53" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="T53" s="1" t="s">
+      <c r="U53" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="U53">
-        <v>3.5</v>
       </c>
     </row>
     <row r="54" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14465,17 +14527,17 @@
       <c r="Q54" s="3">
         <v>1200</v>
       </c>
-      <c r="R54" t="s">
+      <c r="R54" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="S54" t="s">
         <v>68</v>
       </c>
-      <c r="S54" s="4" t="s">
+      <c r="T54" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="T54" s="1">
+      <c r="U54" s="1">
         <v>800</v>
-      </c>
-      <c r="U54">
-        <v>4.5</v>
       </c>
     </row>
     <row r="55" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14530,17 +14592,17 @@
       <c r="Q55" s="3">
         <v>1500</v>
       </c>
-      <c r="R55" t="s">
+      <c r="R55" s="7">
+        <v>3</v>
+      </c>
+      <c r="S55" t="s">
         <v>68</v>
       </c>
-      <c r="S55" s="4" t="s">
+      <c r="T55" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="T55" s="1">
+      <c r="U55" s="1">
         <v>1200</v>
-      </c>
-      <c r="U55">
-        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14595,17 +14657,17 @@
       <c r="Q56" s="3">
         <v>900</v>
       </c>
-      <c r="R56" t="s">
+      <c r="R56" s="7">
+        <v>3</v>
+      </c>
+      <c r="S56" t="s">
         <v>68</v>
       </c>
-      <c r="S56" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="T56" s="1">
+      <c r="T56" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="U56" s="1">
         <v>700</v>
-      </c>
-      <c r="U56">
-        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14660,17 +14722,17 @@
       <c r="Q57" s="3">
         <v>2200</v>
       </c>
-      <c r="R57" t="s">
+      <c r="R57" s="7">
+        <v>3</v>
+      </c>
+      <c r="S57" t="s">
         <v>68</v>
       </c>
-      <c r="S57" s="4" t="s">
+      <c r="T57" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="T57" s="1">
+      <c r="U57" s="1">
         <v>1000</v>
-      </c>
-      <c r="U57">
-        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14725,17 +14787,17 @@
       <c r="Q58" s="3">
         <v>1000</v>
       </c>
-      <c r="R58" t="s">
+      <c r="R58" s="7">
+        <v>3</v>
+      </c>
+      <c r="S58" t="s">
         <v>68</v>
       </c>
-      <c r="S58" s="4" t="s">
+      <c r="T58" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="T58" s="1">
+      <c r="U58" s="1">
         <v>800</v>
-      </c>
-      <c r="U58">
-        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14790,15 +14852,17 @@
       <c r="Q59" s="3">
         <v>300</v>
       </c>
-      <c r="R59" t="s">
+      <c r="R59" s="7">
+        <v>4</v>
+      </c>
+      <c r="S59" t="s">
         <v>68</v>
       </c>
-      <c r="S59" s="4"/>
-      <c r="T59" s="1">
+      <c r="T59" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="U59" s="1">
         <v>700</v>
-      </c>
-      <c r="U59">
-        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14853,15 +14917,17 @@
       <c r="Q60" s="3">
         <v>1800</v>
       </c>
-      <c r="R60" t="s">
+      <c r="R60" s="7">
+        <v>4</v>
+      </c>
+      <c r="S60" t="s">
         <v>68</v>
       </c>
-      <c r="S60" s="4"/>
-      <c r="T60" s="1">
+      <c r="T60" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="U60" s="1">
         <v>1000</v>
-      </c>
-      <c r="U60">
-        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14916,15 +14982,17 @@
       <c r="Q61" s="3">
         <v>500</v>
       </c>
-      <c r="R61" t="s">
+      <c r="R61" s="7">
+        <v>4</v>
+      </c>
+      <c r="S61" t="s">
         <v>68</v>
       </c>
-      <c r="S61" s="4"/>
-      <c r="T61" s="1">
+      <c r="T61" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="U61" s="1">
         <v>800</v>
-      </c>
-      <c r="U61">
-        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -14979,15 +15047,17 @@
       <c r="Q62" s="3">
         <v>800</v>
       </c>
-      <c r="R62" t="s">
+      <c r="R62" s="7">
+        <v>4</v>
+      </c>
+      <c r="S62" t="s">
         <v>68</v>
       </c>
-      <c r="S62" s="4"/>
-      <c r="T62" s="1">
+      <c r="T62" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="U62" s="1">
         <v>500</v>
-      </c>
-      <c r="U62">
-        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -15042,17 +15112,17 @@
       <c r="Q63" s="3">
         <v>1200</v>
       </c>
-      <c r="R63" t="s">
+      <c r="R63" s="7">
+        <v>4</v>
+      </c>
+      <c r="S63" t="s">
         <v>68</v>
       </c>
-      <c r="S63" s="4" t="s">
+      <c r="T63" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="T63" s="1">
+      <c r="U63" s="1">
         <v>700</v>
-      </c>
-      <c r="U63">
-        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -15107,15 +15177,17 @@
       <c r="Q64" s="3">
         <v>600</v>
       </c>
-      <c r="R64" t="s">
+      <c r="R64" s="7">
+        <v>5</v>
+      </c>
+      <c r="S64" t="s">
         <v>68</v>
       </c>
-      <c r="S64" s="4"/>
-      <c r="T64" s="1">
+      <c r="T64" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="U64" s="1">
         <v>700</v>
-      </c>
-      <c r="U64">
-        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -15170,17 +15242,17 @@
       <c r="Q65" s="3">
         <v>900</v>
       </c>
-      <c r="R65" t="s">
+      <c r="R65" s="7">
+        <v>5</v>
+      </c>
+      <c r="S65" t="s">
         <v>68</v>
       </c>
-      <c r="S65" s="4" t="s">
+      <c r="T65" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="T65" s="1">
+      <c r="U65" s="1">
         <v>600</v>
-      </c>
-      <c r="U65">
-        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -15235,15 +15307,17 @@
       <c r="Q66" s="3">
         <v>400</v>
       </c>
-      <c r="R66" t="s">
+      <c r="R66" s="7">
+        <v>5</v>
+      </c>
+      <c r="S66" t="s">
         <v>68</v>
       </c>
-      <c r="S66" s="4"/>
-      <c r="T66" s="1">
+      <c r="T66" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="U66" s="1">
         <v>400</v>
-      </c>
-      <c r="U66">
-        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -15298,17 +15372,17 @@
       <c r="Q67" s="3">
         <v>1500</v>
       </c>
-      <c r="R67" t="s">
+      <c r="R67" s="7">
+        <v>5</v>
+      </c>
+      <c r="S67" t="s">
         <v>68</v>
       </c>
-      <c r="S67" s="4" t="s">
+      <c r="T67" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="T67" s="1">
+      <c r="U67" s="1">
         <v>1000</v>
-      </c>
-      <c r="U67">
-        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -15363,17 +15437,17 @@
       <c r="Q68" s="3">
         <v>700</v>
       </c>
-      <c r="R68" t="s">
+      <c r="R68" s="7">
+        <v>5</v>
+      </c>
+      <c r="S68" t="s">
         <v>68</v>
       </c>
-      <c r="S68" s="4" t="s">
+      <c r="T68" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="T68" s="1">
+      <c r="U68" s="1">
         <v>800</v>
-      </c>
-      <c r="U68">
-        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -15428,17 +15502,17 @@
       <c r="Q69" s="3">
         <v>100</v>
       </c>
-      <c r="R69" t="s">
+      <c r="R69" s="7">
+        <v>5</v>
+      </c>
+      <c r="S69" t="s">
         <v>68</v>
       </c>
-      <c r="S69" s="4" t="s">
+      <c r="T69" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="T69" s="1">
+      <c r="U69" s="1">
         <v>3000</v>
-      </c>
-      <c r="U69">
-        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -15493,17 +15567,17 @@
       <c r="Q70" s="3">
         <v>800</v>
       </c>
-      <c r="R70" t="s">
+      <c r="R70" s="7">
+        <v>5</v>
+      </c>
+      <c r="S70" t="s">
         <v>68</v>
       </c>
-      <c r="S70" s="4" t="s">
+      <c r="T70" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="T70" s="1">
+      <c r="U70" s="1">
         <v>500</v>
-      </c>
-      <c r="U70">
-        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -15558,15 +15632,17 @@
       <c r="Q71" s="3">
         <v>1200</v>
       </c>
-      <c r="R71" t="s">
+      <c r="R71" s="7">
+        <v>5</v>
+      </c>
+      <c r="S71" t="s">
         <v>68</v>
       </c>
-      <c r="S71" s="4"/>
-      <c r="T71" s="1">
+      <c r="T71" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="U71" s="1">
         <v>700</v>
-      </c>
-      <c r="U71">
-        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -15621,17 +15697,17 @@
       <c r="Q72" s="3">
         <v>900</v>
       </c>
-      <c r="R72" t="s">
+      <c r="R72" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="S72" t="s">
         <v>68</v>
       </c>
-      <c r="S72" s="4" t="s">
+      <c r="T72" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="T72" s="1">
+      <c r="U72" s="1">
         <v>600</v>
-      </c>
-      <c r="U72">
-        <v>2.5</v>
       </c>
     </row>
     <row r="73" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -15686,15 +15762,17 @@
       <c r="Q73" s="3">
         <v>300</v>
       </c>
-      <c r="R73" t="s">
+      <c r="R73" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="S73" t="s">
         <v>68</v>
       </c>
-      <c r="S73" s="4"/>
-      <c r="T73" s="1">
+      <c r="T73" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="U73" s="1">
         <v>400</v>
-      </c>
-      <c r="U73">
-        <v>2.5</v>
       </c>
     </row>
     <row r="74" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -15749,15 +15827,17 @@
       <c r="Q74" s="3">
         <v>1000</v>
       </c>
-      <c r="R74" t="s">
+      <c r="R74" s="7">
+        <v>3</v>
+      </c>
+      <c r="S74" t="s">
         <v>68</v>
       </c>
-      <c r="S74" s="4"/>
-      <c r="T74" s="1">
+      <c r="T74" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="U74" s="1">
         <v>800</v>
-      </c>
-      <c r="U74">
-        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -15812,17 +15892,17 @@
       <c r="Q75" s="3">
         <v>200</v>
       </c>
-      <c r="R75" t="s">
+      <c r="R75" s="7">
+        <v>3</v>
+      </c>
+      <c r="S75" t="s">
         <v>68</v>
       </c>
-      <c r="S75" s="4" t="s">
+      <c r="T75" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="T75" s="1">
+      <c r="U75" s="1">
         <v>350</v>
-      </c>
-      <c r="U75">
-        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -15877,17 +15957,17 @@
       <c r="Q76" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R76" t="s">
+      <c r="R76" s="7">
+        <v>3</v>
+      </c>
+      <c r="S76" t="s">
         <v>68</v>
       </c>
-      <c r="S76" s="4" t="s">
+      <c r="T76" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="T76" s="1" t="s">
+      <c r="U76" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="U76">
-        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -15942,17 +16022,17 @@
       <c r="Q77" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="R77" t="s">
+      <c r="R77" s="7">
+        <v>3</v>
+      </c>
+      <c r="S77" t="s">
         <v>68</v>
       </c>
-      <c r="S77" s="4" t="s">
+      <c r="T77" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="T77" s="1" t="s">
+      <c r="U77" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="U77">
-        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16007,15 +16087,17 @@
       <c r="Q78" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="R78" t="s">
+      <c r="R78" s="7">
+        <v>4</v>
+      </c>
+      <c r="S78" t="s">
         <v>68</v>
       </c>
-      <c r="S78" s="4"/>
-      <c r="T78" s="1" t="s">
+      <c r="T78" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="U78" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="U78">
-        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16070,17 +16152,17 @@
       <c r="Q79" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="R79" t="s">
+      <c r="R79" s="7">
+        <v>4</v>
+      </c>
+      <c r="S79" t="s">
         <v>68</v>
       </c>
-      <c r="S79" s="4" t="s">
+      <c r="T79" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="T79" s="1" t="s">
+      <c r="U79" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="U79">
-        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16135,15 +16217,17 @@
       <c r="Q80" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R80" t="s">
+      <c r="R80" s="7">
+        <v>4</v>
+      </c>
+      <c r="S80" t="s">
         <v>68</v>
       </c>
-      <c r="S80" s="4"/>
-      <c r="T80" s="1" t="s">
+      <c r="T80" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="U80" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="U80">
-        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16198,15 +16282,17 @@
       <c r="Q81" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="R81" t="s">
+      <c r="R81" s="7">
+        <v>4</v>
+      </c>
+      <c r="S81" t="s">
         <v>68</v>
       </c>
-      <c r="S81" s="4"/>
-      <c r="T81" s="1" t="s">
+      <c r="T81" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="U81" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="U81">
-        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16261,17 +16347,17 @@
       <c r="Q82" s="3">
         <v>1000</v>
       </c>
-      <c r="R82" t="s">
+      <c r="R82" s="7">
+        <v>4</v>
+      </c>
+      <c r="S82" t="s">
         <v>68</v>
       </c>
-      <c r="S82" s="4" t="s">
+      <c r="T82" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="T82" s="1">
+      <c r="U82" s="1">
         <v>800</v>
-      </c>
-      <c r="U82">
-        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16326,17 +16412,17 @@
       <c r="Q83" s="3">
         <v>1500</v>
       </c>
-      <c r="R83" t="s">
+      <c r="R83" s="7">
+        <v>5</v>
+      </c>
+      <c r="S83" t="s">
         <v>68</v>
       </c>
-      <c r="S83" s="4" t="s">
+      <c r="T83" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="T83" s="1">
+      <c r="U83" s="1">
         <v>1200</v>
-      </c>
-      <c r="U83">
-        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16391,17 +16477,17 @@
       <c r="Q84" s="3">
         <v>300</v>
       </c>
-      <c r="R84" t="s">
+      <c r="R84" s="7">
+        <v>5</v>
+      </c>
+      <c r="S84" t="s">
         <v>68</v>
       </c>
-      <c r="S84" s="4" t="s">
+      <c r="T84" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="T84" s="1">
+      <c r="U84" s="1">
         <v>900</v>
-      </c>
-      <c r="U84">
-        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16456,17 +16542,17 @@
       <c r="Q85" s="3">
         <v>2000</v>
       </c>
-      <c r="R85" t="s">
+      <c r="R85" s="7">
+        <v>5</v>
+      </c>
+      <c r="S85" t="s">
         <v>68</v>
       </c>
-      <c r="S85" s="4" t="s">
+      <c r="T85" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="T85" s="1">
+      <c r="U85" s="1">
         <v>700</v>
-      </c>
-      <c r="U85">
-        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16521,17 +16607,17 @@
       <c r="Q86" s="3">
         <v>200</v>
       </c>
-      <c r="R86" t="s">
+      <c r="R86" s="7">
+        <v>5</v>
+      </c>
+      <c r="S86" t="s">
         <v>68</v>
       </c>
-      <c r="S86" s="4" t="s">
+      <c r="T86" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="T86" s="1">
+      <c r="U86" s="1">
         <v>500</v>
-      </c>
-      <c r="U86">
-        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16586,17 +16672,17 @@
       <c r="Q87" s="3">
         <v>1000</v>
       </c>
-      <c r="R87" t="s">
+      <c r="R87" s="7">
+        <v>5</v>
+      </c>
+      <c r="S87" t="s">
         <v>68</v>
       </c>
-      <c r="S87" s="4" t="s">
+      <c r="T87" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="T87" s="1">
+      <c r="U87" s="1">
         <v>700</v>
-      </c>
-      <c r="U87">
-        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16651,15 +16737,17 @@
       <c r="Q88" s="3">
         <v>800</v>
       </c>
-      <c r="R88" t="s">
+      <c r="R88" s="7">
+        <v>4</v>
+      </c>
+      <c r="S88" t="s">
         <v>68</v>
       </c>
-      <c r="S88" s="4"/>
-      <c r="T88" s="1">
+      <c r="T88" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="U88" s="1">
         <v>1000</v>
-      </c>
-      <c r="U88">
-        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16714,15 +16802,17 @@
       <c r="Q89" s="3">
         <v>500</v>
       </c>
-      <c r="R89" t="s">
+      <c r="R89" s="7">
+        <v>3</v>
+      </c>
+      <c r="S89" t="s">
         <v>68</v>
       </c>
-      <c r="S89" s="4"/>
-      <c r="T89" s="1">
+      <c r="T89" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="U89" s="1">
         <v>800</v>
-      </c>
-      <c r="U89">
-        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16777,17 +16867,17 @@
       <c r="Q90" s="3">
         <v>1300</v>
       </c>
-      <c r="R90" t="s">
+      <c r="R90" s="7">
+        <v>3</v>
+      </c>
+      <c r="S90" t="s">
         <v>68</v>
       </c>
-      <c r="S90" s="4" t="s">
+      <c r="T90" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="T90" s="1">
+      <c r="U90" s="1">
         <v>600</v>
-      </c>
-      <c r="U90">
-        <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16842,17 +16932,17 @@
       <c r="Q91" s="3">
         <v>700</v>
       </c>
-      <c r="R91" t="s">
+      <c r="R91" s="7">
+        <v>3</v>
+      </c>
+      <c r="S91" t="s">
         <v>68</v>
       </c>
-      <c r="S91" s="4" t="s">
+      <c r="T91" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="T91" s="1">
+      <c r="U91" s="1">
         <v>900</v>
-      </c>
-      <c r="U91">
-        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16907,15 +16997,17 @@
       <c r="Q92" s="3">
         <v>1200</v>
       </c>
-      <c r="R92" t="s">
+      <c r="R92" s="7">
+        <v>3</v>
+      </c>
+      <c r="S92" t="s">
         <v>68</v>
       </c>
-      <c r="S92" s="4"/>
-      <c r="T92" s="1">
+      <c r="T92" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="U92" s="1">
         <v>700</v>
-      </c>
-      <c r="U92">
-        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -16970,15 +17062,17 @@
       <c r="Q93" s="3">
         <v>900</v>
       </c>
-      <c r="R93" t="s">
+      <c r="R93" s="7">
+        <v>3</v>
+      </c>
+      <c r="S93" t="s">
         <v>68</v>
       </c>
-      <c r="S93" s="4"/>
-      <c r="T93" s="1">
+      <c r="T93" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="U93" s="1">
         <v>1000</v>
-      </c>
-      <c r="U93">
-        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -17033,17 +17127,17 @@
       <c r="Q94" s="3">
         <v>400</v>
       </c>
-      <c r="R94" t="s">
+      <c r="R94" s="7">
+        <v>4</v>
+      </c>
+      <c r="S94" t="s">
         <v>68</v>
       </c>
-      <c r="S94" s="4" t="s">
+      <c r="T94" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="T94" s="1">
+      <c r="U94" s="1">
         <v>700</v>
-      </c>
-      <c r="U94">
-        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -17098,17 +17192,17 @@
       <c r="Q95" s="3">
         <v>800</v>
       </c>
-      <c r="R95" t="s">
+      <c r="R95" s="7">
+        <v>4</v>
+      </c>
+      <c r="S95" t="s">
         <v>68</v>
       </c>
-      <c r="S95" s="4" t="s">
+      <c r="T95" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="T95" s="1">
+      <c r="U95" s="1">
         <v>800</v>
-      </c>
-      <c r="U95">
-        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -17163,17 +17257,17 @@
       <c r="Q96" s="3">
         <v>5000</v>
       </c>
-      <c r="R96" t="s">
+      <c r="R96" s="7">
+        <v>4</v>
+      </c>
+      <c r="S96" t="s">
         <v>68</v>
       </c>
-      <c r="S96" s="4" t="s">
+      <c r="T96" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="T96" s="1">
+      <c r="U96" s="1">
         <v>2500</v>
-      </c>
-      <c r="U96">
-        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -17228,17 +17322,17 @@
       <c r="Q97" s="3">
         <v>6000</v>
       </c>
-      <c r="R97" t="s">
+      <c r="R97" s="7">
+        <v>4</v>
+      </c>
+      <c r="S97" t="s">
         <v>68</v>
       </c>
-      <c r="S97" s="4" t="s">
+      <c r="T97" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="T97" s="1">
+      <c r="U97" s="1">
         <v>3000</v>
-      </c>
-      <c r="U97">
-        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -17293,17 +17387,17 @@
       <c r="Q98" s="3">
         <v>8000</v>
       </c>
-      <c r="R98" t="s">
+      <c r="R98" s="7">
+        <v>5</v>
+      </c>
+      <c r="S98" t="s">
         <v>68</v>
       </c>
-      <c r="S98" s="4" t="s">
+      <c r="T98" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="T98" s="1">
+      <c r="U98" s="1">
         <v>2500</v>
-      </c>
-      <c r="U98">
-        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -17358,17 +17452,17 @@
       <c r="Q99" s="3">
         <v>5000</v>
       </c>
-      <c r="R99" t="s">
+      <c r="R99" s="7">
+        <v>3</v>
+      </c>
+      <c r="S99" t="s">
         <v>68</v>
       </c>
-      <c r="S99" s="4" t="s">
+      <c r="T99" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="T99" s="1">
+      <c r="U99" s="1">
         <v>3000</v>
-      </c>
-      <c r="U99">
-        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -17423,15 +17517,17 @@
       <c r="Q100" s="3">
         <v>6000</v>
       </c>
-      <c r="R100" t="s">
+      <c r="R100" s="7">
+        <v>5</v>
+      </c>
+      <c r="S100" t="s">
         <v>68</v>
       </c>
-      <c r="S100" s="4"/>
-      <c r="T100" s="1">
+      <c r="T100" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="U100" s="1">
         <v>2500</v>
-      </c>
-      <c r="U100">
-        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -17486,17 +17582,17 @@
       <c r="Q101" s="3">
         <v>700</v>
       </c>
-      <c r="R101" t="s">
+      <c r="R101" s="7">
+        <v>3</v>
+      </c>
+      <c r="S101" t="s">
         <v>32</v>
       </c>
-      <c r="S101" s="4" t="s">
+      <c r="T101" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="T101" s="1">
+      <c r="U101" s="1">
         <v>200</v>
-      </c>
-      <c r="U101">
-        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -17551,17 +17647,17 @@
       <c r="Q102" s="3">
         <v>1200</v>
       </c>
-      <c r="R102" t="s">
+      <c r="R102" s="7">
+        <v>3</v>
+      </c>
+      <c r="S102" t="s">
         <v>32</v>
       </c>
-      <c r="S102" s="4" t="s">
+      <c r="T102" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T102" s="1">
+      <c r="U102" s="1">
         <v>200</v>
-      </c>
-      <c r="U102">
-        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -17616,17 +17712,17 @@
       <c r="Q103" s="3">
         <v>800</v>
       </c>
-      <c r="R103" t="s">
+      <c r="R103" s="7">
+        <v>3</v>
+      </c>
+      <c r="S103" t="s">
         <v>32</v>
       </c>
-      <c r="S103" s="4" t="s">
+      <c r="T103" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="T103" s="1">
+      <c r="U103" s="1">
         <v>100</v>
-      </c>
-      <c r="U103">
-        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -17681,17 +17777,17 @@
       <c r="Q104" s="3">
         <v>900</v>
       </c>
-      <c r="R104" t="s">
+      <c r="R104" s="7">
+        <v>4</v>
+      </c>
+      <c r="S104" t="s">
         <v>32</v>
       </c>
-      <c r="S104" s="4" t="s">
+      <c r="T104" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T104" s="1">
+      <c r="U104" s="1">
         <v>150</v>
-      </c>
-      <c r="U104">
-        <v>4</v>
       </c>
     </row>
     <row r="105" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -17746,17 +17842,17 @@
       <c r="Q105" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="R105" t="s">
+      <c r="R105" s="7">
+        <v>4</v>
+      </c>
+      <c r="S105" t="s">
         <v>32</v>
       </c>
-      <c r="S105" s="4" t="s">
+      <c r="T105" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T105" s="1" t="s">
+      <c r="U105" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="U105">
-        <v>4</v>
       </c>
     </row>
     <row r="106" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -17811,17 +17907,17 @@
       <c r="Q106" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="R106" t="s">
+      <c r="R106" s="7">
+        <v>4</v>
+      </c>
+      <c r="S106" t="s">
         <v>32</v>
       </c>
-      <c r="S106" s="4" t="s">
+      <c r="T106" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T106" s="1" t="s">
+      <c r="U106" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="U106">
-        <v>4</v>
       </c>
     </row>
     <row r="107" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -17876,17 +17972,17 @@
       <c r="Q107" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="R107" t="s">
+      <c r="R107" s="7">
+        <v>4</v>
+      </c>
+      <c r="S107" t="s">
         <v>32</v>
       </c>
-      <c r="S107" s="4" t="s">
+      <c r="T107" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T107" s="1" t="s">
+      <c r="U107" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="U107">
-        <v>4</v>
       </c>
     </row>
     <row r="108" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -17941,17 +18037,17 @@
       <c r="Q108" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="R108" t="s">
+      <c r="R108" s="7">
+        <v>5</v>
+      </c>
+      <c r="S108" t="s">
         <v>32</v>
       </c>
-      <c r="S108" s="4" t="s">
+      <c r="T108" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T108" s="1" t="s">
+      <c r="U108" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="U108">
-        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18006,17 +18102,17 @@
       <c r="Q109" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="R109" t="s">
+      <c r="R109" s="7">
+        <v>5</v>
+      </c>
+      <c r="S109" t="s">
         <v>32</v>
       </c>
-      <c r="S109" s="4" t="s">
+      <c r="T109" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="T109" s="1" t="s">
+      <c r="U109" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="U109">
-        <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18071,17 +18167,17 @@
       <c r="Q110" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="R110" t="s">
+      <c r="R110" s="7">
+        <v>5</v>
+      </c>
+      <c r="S110" t="s">
         <v>32</v>
       </c>
-      <c r="S110" s="4" t="s">
+      <c r="T110" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="T110" s="1" t="s">
+      <c r="U110" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="U110">
-        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18136,17 +18232,17 @@
       <c r="Q111" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="R111" t="s">
+      <c r="R111" s="7">
+        <v>5</v>
+      </c>
+      <c r="S111" t="s">
         <v>32</v>
       </c>
-      <c r="S111" s="4" t="s">
+      <c r="T111" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T111" s="1" t="s">
+      <c r="U111" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="U111">
-        <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18201,17 +18297,17 @@
       <c r="Q112" s="3">
         <v>800</v>
       </c>
-      <c r="R112" t="s">
+      <c r="R112" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="S112" t="s">
         <v>32</v>
       </c>
-      <c r="S112" s="4" t="s">
+      <c r="T112" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T112" s="1">
+      <c r="U112" s="1">
         <v>150</v>
-      </c>
-      <c r="U112">
-        <v>2.5</v>
       </c>
     </row>
     <row r="113" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18266,17 +18362,17 @@
       <c r="Q113" s="3">
         <v>900</v>
       </c>
-      <c r="R113" t="s">
+      <c r="R113" s="7">
+        <v>5</v>
+      </c>
+      <c r="S113" t="s">
         <v>32</v>
       </c>
-      <c r="S113" s="4" t="s">
+      <c r="T113" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T113" s="1">
+      <c r="U113" s="1">
         <v>100</v>
-      </c>
-      <c r="U113">
-        <v>5</v>
       </c>
     </row>
     <row r="114" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18331,17 +18427,17 @@
       <c r="Q114" s="3">
         <v>400</v>
       </c>
-      <c r="R114" t="s">
+      <c r="R114" s="7">
+        <v>5</v>
+      </c>
+      <c r="S114" t="s">
         <v>32</v>
       </c>
-      <c r="S114" s="4" t="s">
+      <c r="T114" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="T114" s="1">
+      <c r="U114" s="1">
         <v>150</v>
-      </c>
-      <c r="U114">
-        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18396,17 +18492,17 @@
       <c r="Q115" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="R115" t="s">
+      <c r="R115" s="7">
+        <v>5</v>
+      </c>
+      <c r="S115" t="s">
         <v>32</v>
       </c>
-      <c r="S115" s="4" t="s">
+      <c r="T115" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T115" s="1" t="s">
+      <c r="U115" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="U115">
-        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18461,17 +18557,17 @@
       <c r="Q116" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="R116" t="s">
+      <c r="R116" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="S116" t="s">
         <v>32</v>
       </c>
-      <c r="S116" s="4" t="s">
+      <c r="T116" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="T116" s="1" t="s">
+      <c r="U116" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="U116">
-        <v>3.5</v>
       </c>
     </row>
     <row r="117" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18526,17 +18622,17 @@
       <c r="Q117" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="R117" t="s">
+      <c r="R117" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="S117" t="s">
         <v>32</v>
       </c>
-      <c r="S117" s="4" t="s">
+      <c r="T117" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T117" s="1" t="s">
+      <c r="U117" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="U117">
-        <v>3.5</v>
       </c>
     </row>
     <row r="118" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18591,17 +18687,17 @@
       <c r="Q118" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R118" t="s">
+      <c r="R118" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="S118" t="s">
         <v>32</v>
       </c>
-      <c r="S118" s="4" t="s">
+      <c r="T118" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="T118" s="1" t="s">
+      <c r="U118" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="U118">
-        <v>4.5</v>
       </c>
     </row>
     <row r="119" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18656,17 +18752,17 @@
       <c r="Q119" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="R119" t="s">
+      <c r="R119" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="S119" t="s">
         <v>32</v>
       </c>
-      <c r="S119" s="4" t="s">
+      <c r="T119" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T119" s="1" t="s">
+      <c r="U119" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="U119">
-        <v>4.5</v>
       </c>
     </row>
     <row r="120" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18721,17 +18817,17 @@
       <c r="Q120" s="3">
         <v>400</v>
       </c>
-      <c r="R120" t="s">
+      <c r="R120" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="S120" t="s">
         <v>32</v>
       </c>
-      <c r="S120" s="4" t="s">
+      <c r="T120" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="T120" s="1">
+      <c r="U120" s="1">
         <v>300</v>
-      </c>
-      <c r="U120">
-        <v>4.5</v>
       </c>
     </row>
     <row r="121" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18786,17 +18882,17 @@
       <c r="Q121" s="3">
         <v>1100</v>
       </c>
-      <c r="R121" t="s">
+      <c r="R121" s="7">
+        <v>3</v>
+      </c>
+      <c r="S121" t="s">
         <v>32</v>
       </c>
-      <c r="S121" s="4" t="s">
+      <c r="T121" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T121" s="1">
+      <c r="U121" s="1">
         <v>200</v>
-      </c>
-      <c r="U121">
-        <v>3</v>
       </c>
     </row>
     <row r="122" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18851,17 +18947,17 @@
       <c r="Q122" s="3">
         <v>1300</v>
       </c>
-      <c r="R122" t="s">
+      <c r="R122" s="7">
+        <v>4</v>
+      </c>
+      <c r="S122" t="s">
         <v>32</v>
       </c>
-      <c r="S122" s="4" t="s">
+      <c r="T122" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T122" s="1">
+      <c r="U122" s="1">
         <v>100</v>
-      </c>
-      <c r="U122">
-        <v>4</v>
       </c>
     </row>
     <row r="123" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18916,17 +19012,17 @@
       <c r="Q123" s="3">
         <v>1000</v>
       </c>
-      <c r="R123" t="s">
+      <c r="R123" s="7">
+        <v>4</v>
+      </c>
+      <c r="S123" t="s">
         <v>32</v>
       </c>
-      <c r="S123" s="4" t="s">
+      <c r="T123" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="T123" s="1">
+      <c r="U123" s="1">
         <v>200</v>
-      </c>
-      <c r="U123">
-        <v>4</v>
       </c>
     </row>
     <row r="124" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -18981,17 +19077,17 @@
       <c r="Q124" s="3">
         <v>500</v>
       </c>
-      <c r="R124" t="s">
+      <c r="R124" s="7">
+        <v>5</v>
+      </c>
+      <c r="S124" t="s">
         <v>32</v>
       </c>
-      <c r="S124" s="4" t="s">
+      <c r="T124" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="T124" s="1">
+      <c r="U124" s="1">
         <v>300</v>
-      </c>
-      <c r="U124">
-        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -19046,17 +19142,17 @@
       <c r="Q125" s="3">
         <v>400</v>
       </c>
-      <c r="R125" t="s">
+      <c r="R125" s="7">
+        <v>3</v>
+      </c>
+      <c r="S125" t="s">
         <v>32</v>
       </c>
-      <c r="S125" s="4" t="s">
+      <c r="T125" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="T125" s="1">
+      <c r="U125" s="1">
         <v>100</v>
-      </c>
-      <c r="U125">
-        <v>3</v>
       </c>
     </row>
     <row r="126" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -19111,17 +19207,17 @@
       <c r="Q126" s="3">
         <v>800</v>
       </c>
-      <c r="R126" t="s">
+      <c r="R126" s="7">
+        <v>3</v>
+      </c>
+      <c r="S126" t="s">
         <v>32</v>
       </c>
-      <c r="S126" s="4" t="s">
+      <c r="T126" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T126" s="1">
+      <c r="U126" s="1">
         <v>150</v>
-      </c>
-      <c r="U126">
-        <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -19176,17 +19272,17 @@
       <c r="Q127" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="R127" t="s">
+      <c r="R127" s="7">
+        <v>3</v>
+      </c>
+      <c r="S127" t="s">
         <v>32</v>
       </c>
-      <c r="S127" s="4" t="s">
+      <c r="T127" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="T127" s="1" t="s">
+      <c r="U127" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="U127">
-        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -19241,17 +19337,17 @@
       <c r="Q128" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="R128" t="s">
+      <c r="R128" s="7">
+        <v>4</v>
+      </c>
+      <c r="S128" t="s">
         <v>32</v>
       </c>
-      <c r="S128" s="4" t="s">
+      <c r="T128" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="T128" s="1" t="s">
+      <c r="U128" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="U128">
-        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -19306,17 +19402,17 @@
       <c r="Q129" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="R129" t="s">
+      <c r="R129" s="7">
+        <v>4</v>
+      </c>
+      <c r="S129" t="s">
         <v>32</v>
       </c>
-      <c r="S129" s="4" t="s">
+      <c r="T129" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T129" s="1" t="s">
+      <c r="U129" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="U129">
-        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -19371,17 +19467,17 @@
       <c r="Q130" s="3">
         <v>800</v>
       </c>
-      <c r="R130" t="s">
+      <c r="R130" s="7">
+        <v>4</v>
+      </c>
+      <c r="S130" t="s">
         <v>32</v>
       </c>
-      <c r="S130" s="4" t="s">
+      <c r="T130" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="T130" s="1">
+      <c r="U130" s="1">
         <v>500</v>
-      </c>
-      <c r="U130">
-        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -19436,17 +19532,17 @@
       <c r="Q131" s="3">
         <v>900</v>
       </c>
-      <c r="R131" t="s">
+      <c r="R131" s="7">
+        <v>5</v>
+      </c>
+      <c r="S131" t="s">
         <v>32</v>
       </c>
-      <c r="S131" s="4" t="s">
+      <c r="T131" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T131" s="1">
+      <c r="U131" s="1">
         <v>150</v>
-      </c>
-      <c r="U131">
-        <v>5</v>
       </c>
     </row>
     <row r="132" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -19501,17 +19597,17 @@
       <c r="Q132" s="3">
         <v>1100</v>
       </c>
-      <c r="R132" t="s">
+      <c r="R132" s="7">
+        <v>5</v>
+      </c>
+      <c r="S132" t="s">
         <v>32</v>
       </c>
-      <c r="S132" s="4" t="s">
+      <c r="T132" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T132" s="1">
+      <c r="U132" s="1">
         <v>250</v>
-      </c>
-      <c r="U132">
-        <v>5</v>
       </c>
     </row>
     <row r="133" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -19566,17 +19662,17 @@
       <c r="Q133" s="3">
         <v>1200</v>
       </c>
-      <c r="R133" t="s">
+      <c r="R133" s="7">
+        <v>5</v>
+      </c>
+      <c r="S133" t="s">
         <v>32</v>
       </c>
-      <c r="S133" s="4" t="s">
+      <c r="T133" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T133" s="1">
+      <c r="U133" s="1">
         <v>500</v>
-      </c>
-      <c r="U133">
-        <v>5</v>
       </c>
     </row>
     <row r="134" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -19631,17 +19727,17 @@
       <c r="Q134" s="3">
         <v>900</v>
       </c>
-      <c r="R134" t="s">
+      <c r="R134" s="7">
+        <v>4</v>
+      </c>
+      <c r="S134" t="s">
         <v>32</v>
       </c>
-      <c r="S134" s="4" t="s">
+      <c r="T134" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T134" s="1">
+      <c r="U134" s="1">
         <v>400</v>
-      </c>
-      <c r="U134">
-        <v>4</v>
       </c>
     </row>
     <row r="135" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -19696,17 +19792,17 @@
       <c r="Q135" s="3">
         <v>7000</v>
       </c>
-      <c r="R135" t="s">
+      <c r="R135" s="7">
+        <v>4</v>
+      </c>
+      <c r="S135" t="s">
         <v>32</v>
       </c>
-      <c r="S135" s="4" t="s">
+      <c r="T135" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="T135" s="1">
+      <c r="U135" s="1">
         <v>1500</v>
-      </c>
-      <c r="U135">
-        <v>4</v>
       </c>
     </row>
     <row r="136" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -19761,17 +19857,17 @@
       <c r="Q136" s="3">
         <v>4000</v>
       </c>
-      <c r="R136" t="s">
+      <c r="R136" s="7">
+        <v>4</v>
+      </c>
+      <c r="S136" t="s">
         <v>32</v>
       </c>
-      <c r="S136" s="4" t="s">
+      <c r="T136" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="T136" s="1">
+      <c r="U136" s="1">
         <v>1500</v>
-      </c>
-      <c r="U136">
-        <v>4</v>
       </c>
     </row>
     <row r="137" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -19826,17 +19922,17 @@
       <c r="Q137" s="3">
         <v>2000</v>
       </c>
-      <c r="R137" t="s">
+      <c r="R137" s="7">
+        <v>2</v>
+      </c>
+      <c r="S137" t="s">
         <v>32</v>
       </c>
-      <c r="S137" s="4" t="s">
+      <c r="T137" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="T137" s="1">
+      <c r="U137" s="1">
         <v>1000</v>
-      </c>
-      <c r="U137">
-        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:21" ht="15" x14ac:dyDescent="0.4">
@@ -19891,22 +19987,22 @@
       <c r="Q138" s="3">
         <v>7000</v>
       </c>
-      <c r="R138" t="s">
+      <c r="R138" s="7">
+        <v>4</v>
+      </c>
+      <c r="S138" t="s">
         <v>32</v>
       </c>
-      <c r="S138" s="4" t="s">
+      <c r="T138" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="T138" s="1">
+      <c r="U138" s="1">
         <v>2500</v>
       </c>
-      <c r="U138">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U139">
-    <sortCondition ref="R47:R139"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V139">
+    <sortCondition ref="S47:S139"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>